<commit_message>
change class labels in tukey input
</commit_message>
<xml_diff>
--- a/tukey_headers.xlsx
+++ b/tukey_headers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noellepatterson/apps/FFC_QA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C01C7573-B8F4-3248-9BAF-C58C40D78771}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A64301B-6560-6243-AADB-5F3731B64F09}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16200" xr2:uid="{A58FFE20-4D46-D149-8BB4-36D0C0EE21A5}"/>
+    <workbookView xWindow="2240" yWindow="4820" windowWidth="18800" windowHeight="11720" xr2:uid="{A58FFE20-4D46-D149-8BB4-36D0C0EE21A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>groups</t>
   </si>
@@ -59,10 +54,16 @@
     <t>Wet_BFL_Mag</t>
   </si>
   <si>
-    <t>Peak_Fre_2</t>
-  </si>
-  <si>
-    <t>Peak_Dur_5</t>
+    <t>Peak_Fre_10</t>
+  </si>
+  <si>
+    <t>Peak_Fre_20</t>
+  </si>
+  <si>
+    <t>Peak_Dur_2</t>
+  </si>
+  <si>
+    <t>Peak_Tim_2</t>
   </si>
 </sst>
 </file>
@@ -414,15 +415,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938FFBD3-6B59-0A40-B758-8D61CCC3F43D}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,6 +456,12 @@
       </c>
       <c r="K1" t="s">
         <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>